<commit_message>
final updated september file
</commit_message>
<xml_diff>
--- a/data/Production_Filled_September.xlsx
+++ b/data/Production_Filled_September.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -655,34 +655,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -708,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -812,9 +784,6 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -851,13 +820,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6979,9 +6945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD11" sqref="AD11:AD12"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR34" sqref="AR34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9828,8 +9794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12031,11 +11997,11 @@
       </c>
     </row>
     <row r="33" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
@@ -12211,11 +12177,11 @@
       </c>
     </row>
     <row r="38" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
@@ -12815,11 +12781,11 @@
       <c r="C50" s="38"/>
     </row>
     <row r="52" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="49"/>
-      <c r="C52" s="49"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="62"/>
       <c r="D52" s="26"/>
       <c r="E52" s="26"/>
       <c r="F52" s="36"/>
@@ -14023,11 +13989,11 @@
       <c r="Y74" s="26"/>
     </row>
     <row r="75" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="B75" s="49"/>
-      <c r="C75" s="49"/>
+      <c r="B75" s="62"/>
+      <c r="C75" s="62"/>
       <c r="D75" s="26"/>
       <c r="E75" s="26"/>
       <c r="F75" s="26"/>
@@ -15217,8 +15183,7 @@
   <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD9" sqref="AD9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15273,13 +15238,13 @@
       <c r="O1" s="48">
         <v>45916</v>
       </c>
-      <c r="P1" s="53">
+      <c r="P1" s="52">
         <v>45917</v>
       </c>
       <c r="Q1" s="48">
         <v>45918</v>
       </c>
-      <c r="R1" s="54">
+      <c r="R1" s="53">
         <v>45920</v>
       </c>
       <c r="S1" s="48">
@@ -15356,37 +15321,37 @@
       <c r="O2" s="32">
         <v>144.5</v>
       </c>
-      <c r="P2" s="50">
+      <c r="P2" s="49">
         <v>146</v>
       </c>
-      <c r="Q2" s="58">
+      <c r="Q2" s="57">
         <v>146</v>
       </c>
-      <c r="R2" s="55">
+      <c r="R2" s="54">
         <v>146</v>
       </c>
-      <c r="S2" s="56">
+      <c r="S2" s="55">
         <v>145</v>
       </c>
-      <c r="T2" s="57">
+      <c r="T2" s="56">
         <v>146</v>
       </c>
-      <c r="U2" s="56">
+      <c r="U2" s="55">
         <v>146</v>
       </c>
-      <c r="V2" s="56">
+      <c r="V2" s="55">
         <v>146</v>
       </c>
-      <c r="W2" s="56">
+      <c r="W2" s="55">
         <v>146</v>
       </c>
-      <c r="X2" s="56">
+      <c r="X2" s="55">
         <v>146</v>
       </c>
-      <c r="Y2" s="56">
+      <c r="Y2" s="55">
         <v>146</v>
       </c>
-      <c r="Z2" s="56">
+      <c r="Z2" s="55">
         <v>146</v>
       </c>
       <c r="AA2" s="32">
@@ -15439,13 +15404,13 @@
       <c r="O3" s="12">
         <v>1.78</v>
       </c>
-      <c r="P3" s="51">
+      <c r="P3" s="50">
         <v>1.78</v>
       </c>
-      <c r="Q3" s="59">
+      <c r="Q3" s="58">
         <v>1.8</v>
       </c>
-      <c r="R3" s="52">
+      <c r="R3" s="51">
         <v>1.76</v>
       </c>
       <c r="S3" s="12">
@@ -15522,13 +15487,13 @@
       <c r="O4" s="12">
         <v>1.1299999999999999</v>
       </c>
-      <c r="P4" s="51">
+      <c r="P4" s="50">
         <v>1.1200000000000001</v>
       </c>
-      <c r="Q4" s="59">
+      <c r="Q4" s="58">
         <v>1.135</v>
       </c>
-      <c r="R4" s="52">
+      <c r="R4" s="51">
         <v>0.54500000000000004</v>
       </c>
       <c r="S4" s="12">
@@ -15549,9 +15514,15 @@
       <c r="X4" s="12">
         <v>0.19</v>
       </c>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
+      <c r="Y4" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
@@ -15599,13 +15570,13 @@
       <c r="O5" s="12">
         <v>0.65</v>
       </c>
-      <c r="P5" s="51">
+      <c r="P5" s="50">
         <v>0.63800000000000001</v>
       </c>
       <c r="Q5" s="39">
         <v>0.64500000000000002</v>
       </c>
-      <c r="R5" s="52">
+      <c r="R5" s="51">
         <v>0.64400000000000002</v>
       </c>
       <c r="S5" s="12">
@@ -15682,13 +15653,13 @@
       <c r="O6" s="12">
         <v>16.693999999999999</v>
       </c>
-      <c r="P6" s="51">
+      <c r="P6" s="50">
         <v>17.187999999999999</v>
       </c>
-      <c r="Q6" s="60">
+      <c r="Q6" s="59">
         <v>17.263999999999999</v>
       </c>
-      <c r="R6" s="52">
+      <c r="R6" s="51">
         <v>17.088999999999999</v>
       </c>
       <c r="S6" s="12">
@@ -15765,20 +15736,42 @@
       <c r="O7" s="12">
         <v>0</v>
       </c>
-      <c r="P7" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
-      <c r="AA7" s="12"/>
+      <c r="P7" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>0</v>
+      </c>
+      <c r="R7" s="12">
+        <v>0</v>
+      </c>
+      <c r="S7" s="12">
+        <v>0</v>
+      </c>
+      <c r="T7" s="12">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12">
+        <v>0</v>
+      </c>
+      <c r="V7" s="12">
+        <v>0</v>
+      </c>
+      <c r="W7" s="12">
+        <v>0</v>
+      </c>
+      <c r="X7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -15826,20 +15819,42 @@
       <c r="O8" s="12">
         <v>0</v>
       </c>
-      <c r="P8" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="61"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="12"/>
+      <c r="P8" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>0</v>
+      </c>
+      <c r="R8" s="12">
+        <v>0</v>
+      </c>
+      <c r="S8" s="12">
+        <v>0</v>
+      </c>
+      <c r="T8" s="12">
+        <v>0</v>
+      </c>
+      <c r="U8" s="12">
+        <v>0</v>
+      </c>
+      <c r="V8" s="12">
+        <v>0</v>
+      </c>
+      <c r="W8" s="12">
+        <v>0</v>
+      </c>
+      <c r="X8" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
@@ -15887,13 +15902,13 @@
       <c r="O9" s="12">
         <v>0</v>
       </c>
-      <c r="P9" s="51">
+      <c r="P9" s="50">
         <v>1.8</v>
       </c>
-      <c r="Q9" s="62">
-        <v>0</v>
-      </c>
-      <c r="R9" s="52">
+      <c r="Q9" s="60">
+        <v>0</v>
+      </c>
+      <c r="R9" s="51">
         <v>2.1</v>
       </c>
       <c r="S9" s="12">
@@ -15905,14 +15920,24 @@
       <c r="U9" s="12">
         <v>0</v>
       </c>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
+      <c r="V9" s="12">
+        <v>0</v>
+      </c>
+      <c r="W9" s="12">
+        <v>0</v>
+      </c>
       <c r="X9" s="12">
         <v>1.89</v>
       </c>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="12"/>
-      <c r="AA9" s="12"/>
+      <c r="Y9" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -15960,13 +15985,13 @@
       <c r="O10" s="12">
         <v>10.843999999999999</v>
       </c>
-      <c r="P10" s="51">
+      <c r="P10" s="50">
         <v>10.638</v>
       </c>
       <c r="Q10" s="12">
         <v>10.28</v>
       </c>
-      <c r="R10" s="52">
+      <c r="R10" s="51">
         <v>9.39</v>
       </c>
       <c r="S10" s="12">
@@ -16043,13 +16068,13 @@
       <c r="O11" s="12">
         <v>3.99</v>
       </c>
-      <c r="P11" s="51">
+      <c r="P11" s="50">
         <v>3.97</v>
       </c>
       <c r="Q11" s="39">
         <v>3.98</v>
       </c>
-      <c r="R11" s="52">
+      <c r="R11" s="51">
         <v>3.86</v>
       </c>
       <c r="S11" s="12">
@@ -16126,13 +16151,13 @@
       <c r="O12" s="12">
         <v>5.87</v>
       </c>
-      <c r="P12" s="51">
+      <c r="P12" s="50">
         <v>3.82</v>
       </c>
-      <c r="Q12" s="60">
+      <c r="Q12" s="59">
         <v>5.69</v>
       </c>
-      <c r="R12" s="52">
+      <c r="R12" s="51">
         <v>4.4050000000000002</v>
       </c>
       <c r="S12" s="12">
@@ -16209,20 +16234,42 @@
       <c r="O13" s="12">
         <v>0</v>
       </c>
-      <c r="P13" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="62"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
+      <c r="P13" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="50">
+        <v>0</v>
+      </c>
+      <c r="R13" s="50">
+        <v>0</v>
+      </c>
+      <c r="S13" s="50">
+        <v>0</v>
+      </c>
+      <c r="T13" s="50">
+        <v>0</v>
+      </c>
+      <c r="U13" s="50">
+        <v>0</v>
+      </c>
+      <c r="V13" s="50">
+        <v>0</v>
+      </c>
+      <c r="W13" s="50">
+        <v>0</v>
+      </c>
+      <c r="X13" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -16270,13 +16317,13 @@
       <c r="O14" s="12">
         <v>0</v>
       </c>
-      <c r="P14" s="51">
+      <c r="P14" s="50">
         <v>0</v>
       </c>
       <c r="Q14" s="12">
         <v>0.27</v>
       </c>
-      <c r="R14" s="52">
+      <c r="R14" s="51">
         <v>0.52</v>
       </c>
       <c r="S14" s="12">
@@ -16353,20 +16400,42 @@
       <c r="O15" s="12">
         <v>0</v>
       </c>
-      <c r="P15" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="52"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
+      <c r="P15" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="50">
+        <v>0</v>
+      </c>
+      <c r="R15" s="50">
+        <v>0</v>
+      </c>
+      <c r="S15" s="50">
+        <v>0</v>
+      </c>
+      <c r="T15" s="50">
+        <v>0</v>
+      </c>
+      <c r="U15" s="50">
+        <v>0</v>
+      </c>
+      <c r="V15" s="50">
+        <v>0</v>
+      </c>
+      <c r="W15" s="50">
+        <v>0</v>
+      </c>
+      <c r="X15" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -16414,20 +16483,42 @@
       <c r="O16" s="12">
         <v>0</v>
       </c>
-      <c r="P16" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="61"/>
-      <c r="R16" s="52"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
+      <c r="P16" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="50">
+        <v>0</v>
+      </c>
+      <c r="R16" s="50">
+        <v>0</v>
+      </c>
+      <c r="S16" s="50">
+        <v>0</v>
+      </c>
+      <c r="T16" s="50">
+        <v>0</v>
+      </c>
+      <c r="U16" s="50">
+        <v>0</v>
+      </c>
+      <c r="V16" s="50">
+        <v>0</v>
+      </c>
+      <c r="W16" s="50">
+        <v>0</v>
+      </c>
+      <c r="X16" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -16475,20 +16566,42 @@
       <c r="O17" s="12">
         <v>0</v>
       </c>
-      <c r="P17" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
+      <c r="P17" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="50">
+        <v>0</v>
+      </c>
+      <c r="R17" s="50">
+        <v>0</v>
+      </c>
+      <c r="S17" s="50">
+        <v>0</v>
+      </c>
+      <c r="T17" s="50">
+        <v>0</v>
+      </c>
+      <c r="U17" s="50">
+        <v>0</v>
+      </c>
+      <c r="V17" s="50">
+        <v>0</v>
+      </c>
+      <c r="W17" s="50">
+        <v>0</v>
+      </c>
+      <c r="X17" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -16536,13 +16649,13 @@
       <c r="O18" s="12">
         <v>3.2749999999999999</v>
       </c>
-      <c r="P18" s="51">
+      <c r="P18" s="50">
         <v>3.28</v>
       </c>
-      <c r="Q18" s="64">
+      <c r="Q18" s="61">
         <v>3.54</v>
       </c>
-      <c r="R18" s="52">
+      <c r="R18" s="51">
         <v>4.47</v>
       </c>
       <c r="S18" s="12">
@@ -16619,13 +16732,13 @@
       <c r="O19" s="12">
         <v>0.95499999999999996</v>
       </c>
-      <c r="P19" s="51">
+      <c r="P19" s="50">
         <v>0.92</v>
       </c>
-      <c r="Q19" s="59">
+      <c r="Q19" s="58">
         <v>0.94</v>
       </c>
-      <c r="R19" s="52">
+      <c r="R19" s="51">
         <v>0.88</v>
       </c>
       <c r="S19" s="12">
@@ -16666,8 +16779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16852,8 +16965,8 @@
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q16" sqref="Q16"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17466,8 +17579,7 @@
   <dimension ref="A1:AA18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R13" sqref="R13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17691,17 +17803,39 @@
       <c r="P3" s="12">
         <v>0</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
+      <c r="Q3" s="12">
+        <v>0</v>
+      </c>
+      <c r="R3" s="12">
+        <v>0</v>
+      </c>
+      <c r="S3" s="12">
+        <v>0</v>
+      </c>
+      <c r="T3" s="12">
+        <v>0</v>
+      </c>
+      <c r="U3" s="12">
+        <v>0</v>
+      </c>
+      <c r="V3" s="12">
+        <v>0</v>
+      </c>
+      <c r="W3" s="12">
+        <v>0</v>
+      </c>
+      <c r="X3" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -18250,17 +18384,39 @@
       <c r="P10" s="12">
         <v>0</v>
       </c>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="12"/>
+      <c r="Q10" s="12">
+        <v>0</v>
+      </c>
+      <c r="R10" s="12">
+        <v>0</v>
+      </c>
+      <c r="S10" s="12">
+        <v>0</v>
+      </c>
+      <c r="T10" s="12">
+        <v>0</v>
+      </c>
+      <c r="U10" s="12">
+        <v>0</v>
+      </c>
+      <c r="V10" s="12">
+        <v>0</v>
+      </c>
+      <c r="W10" s="12">
+        <v>0</v>
+      </c>
+      <c r="X10" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -18477,17 +18633,39 @@
       <c r="P13" s="12">
         <v>0</v>
       </c>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
+      <c r="Q13" s="12">
+        <v>0</v>
+      </c>
+      <c r="R13" s="12">
+        <v>0</v>
+      </c>
+      <c r="S13" s="12">
+        <v>0</v>
+      </c>
+      <c r="T13" s="12">
+        <v>0</v>
+      </c>
+      <c r="U13" s="12">
+        <v>0</v>
+      </c>
+      <c r="V13" s="12">
+        <v>0</v>
+      </c>
+      <c r="W13" s="12">
+        <v>0</v>
+      </c>
+      <c r="X13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -18621,17 +18799,39 @@
       <c r="P15" s="12">
         <v>0</v>
       </c>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="12"/>
+      <c r="Q15" s="12">
+        <v>0</v>
+      </c>
+      <c r="R15" s="12">
+        <v>0</v>
+      </c>
+      <c r="S15" s="12">
+        <v>0</v>
+      </c>
+      <c r="T15" s="12">
+        <v>0</v>
+      </c>
+      <c r="U15" s="12">
+        <v>0</v>
+      </c>
+      <c r="V15" s="12">
+        <v>0</v>
+      </c>
+      <c r="W15" s="12">
+        <v>0</v>
+      </c>
+      <c r="X15" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -18811,9 +19011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>